<commit_message>
Test Documents and Changes to View
</commit_message>
<xml_diff>
--- a/UploadMulti/static/Excel_Files/Features.xlsx
+++ b/UploadMulti/static/Excel_Files/Features.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -349,112 +345,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Employee Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Address of Employee</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Company Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Address of Company</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Role</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Base Salary</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Date of Agreement</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Start Date</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>End Date</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Supervisor Information</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Bonus</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Notice Period</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Other Compensation</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Non Monetary Benefits</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Health Insurance</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>401k</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>At will</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Stock</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Vacation</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>